<commit_message>
Adicionado scaffold e seeds para Projects
</commit_message>
<xml_diff>
--- a/Seeds/seeds.xlsx
+++ b/Seeds/seeds.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="School" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Course" sheetId="2" r:id="rId4"/>
     <sheet name="Discipline" sheetId="5" r:id="rId5"/>
     <sheet name="CourseDiscipline" sheetId="7" r:id="rId6"/>
-    <sheet name="Base" sheetId="3" r:id="rId7"/>
+    <sheet name="Project" sheetId="8" r:id="rId7"/>
+    <sheet name="Base" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6195" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6404" uniqueCount="514">
   <si>
     <t>name</t>
   </si>
@@ -1461,6 +1462,117 @@
   </si>
   <si>
     <t xml:space="preserve"> &lt;&lt; </t>
+  </si>
+  <si>
+    <t>grade</t>
+  </si>
+  <si>
+    <t>project1</t>
+  </si>
+  <si>
+    <t>Descr Proj 1</t>
+  </si>
+  <si>
+    <t>Prj1</t>
+  </si>
+  <si>
+    <t>project2</t>
+  </si>
+  <si>
+    <t>Prj2</t>
+  </si>
+  <si>
+    <t>Descr Proj 2</t>
+  </si>
+  <si>
+    <t>project3</t>
+  </si>
+  <si>
+    <t>Prj3</t>
+  </si>
+  <si>
+    <t>Descr Proj 3</t>
+  </si>
+  <si>
+    <t>project4</t>
+  </si>
+  <si>
+    <t>Prj4</t>
+  </si>
+  <si>
+    <t>Descr Proj 4</t>
+  </si>
+  <si>
+    <t>project5</t>
+  </si>
+  <si>
+    <t>Prj5</t>
+  </si>
+  <si>
+    <t>Descr Proj 5</t>
+  </si>
+  <si>
+    <t>project6</t>
+  </si>
+  <si>
+    <t>Prj6</t>
+  </si>
+  <si>
+    <t>Descr Proj 6</t>
+  </si>
+  <si>
+    <t>project7</t>
+  </si>
+  <si>
+    <t>Prj7</t>
+  </si>
+  <si>
+    <t>Descr Proj 7</t>
+  </si>
+  <si>
+    <t>project8</t>
+  </si>
+  <si>
+    <t>Prj8</t>
+  </si>
+  <si>
+    <t>Descr Proj 8</t>
+  </si>
+  <si>
+    <t>project9</t>
+  </si>
+  <si>
+    <t>Prj9</t>
+  </si>
+  <si>
+    <t>Descr Proj 9</t>
+  </si>
+  <si>
+    <t>project10</t>
+  </si>
+  <si>
+    <t>Prj10</t>
+  </si>
+  <si>
+    <t>Descr Proj 10</t>
+  </si>
+  <si>
+    <t>project11</t>
+  </si>
+  <si>
+    <t>Prj11</t>
+  </si>
+  <si>
+    <t>Descr Proj 11</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>discipline</t>
+  </si>
+  <si>
+    <t>Project</t>
   </si>
 </sst>
 </file>
@@ -1534,7 +1646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1548,6 +1660,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5757,7 +5870,7 @@
       </c>
       <c r="J2" s="5" t="str">
         <f ca="1">IF(RAND()&lt;0.5,"True","False")</f>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>1</v>
@@ -5770,14 +5883,14 @@
       </c>
       <c r="N2" s="8">
         <f ca="1">RANDBETWEEN(15,30)</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P2" t="str">
         <f ca="1">IF(ISBLANK(F2),"",CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2))</f>
-        <v>@s1.rooms.create(description:'A100',projector:'True',seats:'19')</v>
+        <v>@s1.rooms.create(description:'A100',projector:'False',seats:'18')</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -5810,7 +5923,7 @@
       </c>
       <c r="J3" s="5" t="str">
         <f t="shared" ref="J3:J65" ca="1" si="0">IF(RAND()&lt;0.5,"True","False")</f>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>1</v>
@@ -5823,14 +5936,14 @@
       </c>
       <c r="N3" s="8">
         <f t="shared" ref="N3:N65" ca="1" si="1">RANDBETWEEN(15,30)</f>
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P3" t="str">
         <f t="shared" ref="P3:P49" ca="1" si="2">IF(ISBLANK(F3),"",CONCATENATE(A3,B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3,M3,N3,O3))</f>
-        <v>@s1.rooms.create(description:'A101',projector:'True',seats:'24')</v>
+        <v>@s1.rooms.create(description:'A101',projector:'False',seats:'18')</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -5863,7 +5976,7 @@
       </c>
       <c r="J4" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>1</v>
@@ -5876,14 +5989,14 @@
       </c>
       <c r="N4" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="O4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A102',projector:'False',seats:'16')</v>
+        <v>@s1.rooms.create(description:'A102',projector:'True',seats:'28')</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -5929,14 +6042,14 @@
       </c>
       <c r="N5" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="O5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A103',projector:'True',seats:'26')</v>
+        <v>@s1.rooms.create(description:'A103',projector:'True',seats:'20')</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -5969,7 +6082,7 @@
       </c>
       <c r="J6" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>1</v>
@@ -5982,14 +6095,14 @@
       </c>
       <c r="N6" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="O6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A104',projector:'True',seats:'16')</v>
+        <v>@s1.rooms.create(description:'A104',projector:'False',seats:'23')</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -6022,7 +6135,7 @@
       </c>
       <c r="J7" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>1</v>
@@ -6042,7 +6155,7 @@
       </c>
       <c r="P7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A105',projector:'False',seats:'27')</v>
+        <v>@s1.rooms.create(description:'A105',projector:'True',seats:'27')</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -6088,14 +6201,14 @@
       </c>
       <c r="N8" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="O8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A106',projector:'True',seats:'28')</v>
+        <v>@s1.rooms.create(description:'A106',projector:'True',seats:'18')</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -6128,7 +6241,7 @@
       </c>
       <c r="J9" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>1</v>
@@ -6141,14 +6254,14 @@
       </c>
       <c r="N9" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="O9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P9" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A107',projector:'True',seats:'22')</v>
+        <v>@s1.rooms.create(description:'A107',projector:'False',seats:'16')</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -6194,14 +6307,14 @@
       </c>
       <c r="N10" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="O10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P10" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A108',projector:'False',seats:'15')</v>
+        <v>@s1.rooms.create(description:'A108',projector:'False',seats:'17')</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -6247,14 +6360,14 @@
       </c>
       <c r="N11" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="O11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A109',projector:'False',seats:'28')</v>
+        <v>@s1.rooms.create(description:'A109',projector:'False',seats:'21')</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -6300,14 +6413,14 @@
       </c>
       <c r="N12" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="O12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P12" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A110',projector:'True',seats:'24')</v>
+        <v>@s1.rooms.create(description:'A110',projector:'True',seats:'17')</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -6340,7 +6453,7 @@
       </c>
       <c r="J13" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>1</v>
@@ -6353,14 +6466,14 @@
       </c>
       <c r="N13" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="O13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P13" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A111',projector:'True',seats:'22')</v>
+        <v>@s1.rooms.create(description:'A111',projector:'False',seats:'17')</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -6406,14 +6519,14 @@
       </c>
       <c r="N14" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="O14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P14" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A112',projector:'True',seats:'28')</v>
+        <v>@s1.rooms.create(description:'A112',projector:'True',seats:'22')</v>
       </c>
       <c r="Q14" s="6"/>
     </row>
@@ -6460,14 +6573,14 @@
       </c>
       <c r="N15" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="O15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P15" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A113',projector:'False',seats:'27')</v>
+        <v>@s1.rooms.create(description:'A113',projector:'False',seats:'15')</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -6500,7 +6613,7 @@
       </c>
       <c r="J16" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>1</v>
@@ -6513,14 +6626,14 @@
       </c>
       <c r="N16" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O16" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A114',projector:'True',seats:'27')</v>
+        <v>@s1.rooms.create(description:'A114',projector:'False',seats:'26')</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -6553,7 +6666,7 @@
       </c>
       <c r="J17" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>1</v>
@@ -6566,14 +6679,14 @@
       </c>
       <c r="N17" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="O17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P17" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A115',projector:'True',seats:'19')</v>
+        <v>@s1.rooms.create(description:'A115',projector:'False',seats:'26')</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -6606,7 +6719,7 @@
       </c>
       <c r="J18" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>1</v>
@@ -6619,14 +6732,14 @@
       </c>
       <c r="N18" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="O18" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P18" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A116',projector:'True',seats:'25')</v>
+        <v>@s1.rooms.create(description:'A116',projector:'False',seats:'16')</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -6672,14 +6785,14 @@
       </c>
       <c r="N19" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="O19" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P19" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A117',projector:'False',seats:'24')</v>
+        <v>@s1.rooms.create(description:'A117',projector:'False',seats:'16')</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -6712,7 +6825,7 @@
       </c>
       <c r="J20" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>1</v>
@@ -6725,14 +6838,14 @@
       </c>
       <c r="N20" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="O20" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P20" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A118',projector:'False',seats:'30')</v>
+        <v>@s1.rooms.create(description:'A118',projector:'True',seats:'15')</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -6765,7 +6878,7 @@
       </c>
       <c r="J21" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>1</v>
@@ -6778,14 +6891,14 @@
       </c>
       <c r="N21" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O21" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A119',projector:'True',seats:'22')</v>
+        <v>@s1.rooms.create(description:'A119',projector:'False',seats:'15')</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -6818,7 +6931,7 @@
       </c>
       <c r="J22" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>1</v>
@@ -6831,14 +6944,14 @@
       </c>
       <c r="N22" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="O22" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A120',projector:'True',seats:'29')</v>
+        <v>@s1.rooms.create(description:'A120',projector:'False',seats:'19')</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -6871,7 +6984,7 @@
       </c>
       <c r="J23" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>1</v>
@@ -6891,7 +7004,7 @@
       </c>
       <c r="P23" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A121',projector:'False',seats:'23')</v>
+        <v>@s1.rooms.create(description:'A121',projector:'True',seats:'23')</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -6937,14 +7050,14 @@
       </c>
       <c r="N24" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="O24" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P24" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A122',projector:'True',seats:'24')</v>
+        <v>@s1.rooms.create(description:'A122',projector:'True',seats:'15')</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -6977,7 +7090,7 @@
       </c>
       <c r="J25" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>1</v>
@@ -6990,14 +7103,14 @@
       </c>
       <c r="N25" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O25" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P25" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A123',projector:'False',seats:'26')</v>
+        <v>@s1.rooms.create(description:'A123',projector:'True',seats:'25')</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -7043,14 +7156,14 @@
       </c>
       <c r="N26" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="O26" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A124',projector:'False',seats:'30')</v>
+        <v>@s1.rooms.create(description:'A124',projector:'False',seats:'18')</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -7149,14 +7262,14 @@
       </c>
       <c r="N28" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="O28" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P28" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A126',projector:'False',seats:'25')</v>
+        <v>@s1.rooms.create(description:'A126',projector:'False',seats:'17')</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -7202,14 +7315,14 @@
       </c>
       <c r="N29" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O29" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P29" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A127',projector:'False',seats:'24')</v>
+        <v>@s1.rooms.create(description:'A127',projector:'False',seats:'21')</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -7242,7 +7355,7 @@
       </c>
       <c r="J30" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>1</v>
@@ -7255,14 +7368,14 @@
       </c>
       <c r="N30" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O30" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P30" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A128',projector:'False',seats:'29')</v>
+        <v>@s1.rooms.create(description:'A128',projector:'True',seats:'28')</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -7308,14 +7421,14 @@
       </c>
       <c r="N31" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O31" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P31" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A129',projector:'False',seats:'19')</v>
+        <v>@s1.rooms.create(description:'A129',projector:'False',seats:'18')</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -7361,14 +7474,14 @@
       </c>
       <c r="N32" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O32" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P32" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A130',projector:'True',seats:'20')</v>
+        <v>@s1.rooms.create(description:'A130',projector:'True',seats:'19')</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -7401,7 +7514,7 @@
       </c>
       <c r="J33" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>1</v>
@@ -7414,14 +7527,14 @@
       </c>
       <c r="N33" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O33" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A131',projector:'True',seats:'25')</v>
+        <v>@s1.rooms.create(description:'A131',projector:'False',seats:'27')</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -7467,14 +7580,14 @@
       </c>
       <c r="N34" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="O34" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P34" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A132',projector:'False',seats:'17')</v>
+        <v>@s1.rooms.create(description:'A132',projector:'False',seats:'24')</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -7507,7 +7620,7 @@
       </c>
       <c r="J35" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>1</v>
@@ -7520,14 +7633,14 @@
       </c>
       <c r="N35" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="O35" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P35" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A133',projector:'False',seats:'17')</v>
+        <v>@s1.rooms.create(description:'A133',projector:'True',seats:'15')</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -7560,7 +7673,7 @@
       </c>
       <c r="J36" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>1</v>
@@ -7573,14 +7686,14 @@
       </c>
       <c r="N36" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="O36" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A134',projector:'False',seats:'19')</v>
+        <v>@s1.rooms.create(description:'A134',projector:'True',seats:'15')</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -7626,14 +7739,14 @@
       </c>
       <c r="N37" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="O37" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P37" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A135',projector:'False',seats:'16')</v>
+        <v>@s1.rooms.create(description:'A135',projector:'False',seats:'26')</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -7679,14 +7792,14 @@
       </c>
       <c r="N38" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O38" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P38" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A136',projector:'True',seats:'21')</v>
+        <v>@s1.rooms.create(description:'A136',projector:'True',seats:'19')</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -7719,7 +7832,7 @@
       </c>
       <c r="J39" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>1</v>
@@ -7732,14 +7845,14 @@
       </c>
       <c r="N39" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="O39" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P39" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A137',projector:'True',seats:'27')</v>
+        <v>@s1.rooms.create(description:'A137',projector:'False',seats:'22')</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -7785,14 +7898,14 @@
       </c>
       <c r="N40" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="O40" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P40" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A138',projector:'False',seats:'30')</v>
+        <v>@s1.rooms.create(description:'A138',projector:'False',seats:'24')</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -7838,14 +7951,14 @@
       </c>
       <c r="N41" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="O41" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P41" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A139',projector:'False',seats:'27')</v>
+        <v>@s1.rooms.create(description:'A139',projector:'False',seats:'15')</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -7891,14 +8004,14 @@
       </c>
       <c r="N42" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="O42" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P42" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A140',projector:'False',seats:'20')</v>
+        <v>@s1.rooms.create(description:'A140',projector:'False',seats:'15')</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -7931,7 +8044,7 @@
       </c>
       <c r="J43" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>1</v>
@@ -7944,14 +8057,14 @@
       </c>
       <c r="N43" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="O43" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P43" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A141',projector:'True',seats:'28')</v>
+        <v>@s1.rooms.create(description:'A141',projector:'False',seats:'25')</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -7984,7 +8097,7 @@
       </c>
       <c r="J44" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>1</v>
@@ -7997,14 +8110,14 @@
       </c>
       <c r="N44" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="O44" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P44" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A142',projector:'True',seats:'26')</v>
+        <v>@s1.rooms.create(description:'A142',projector:'False',seats:'17')</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -8037,7 +8150,7 @@
       </c>
       <c r="J45" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>1</v>
@@ -8050,14 +8163,14 @@
       </c>
       <c r="N45" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="O45" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P45" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A143',projector:'False',seats:'19')</v>
+        <v>@s1.rooms.create(description:'A143',projector:'True',seats:'25')</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -8103,14 +8216,14 @@
       </c>
       <c r="N46" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="O46" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P46" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A144',projector:'False',seats:'20')</v>
+        <v>@s1.rooms.create(description:'A144',projector:'False',seats:'18')</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -8143,7 +8256,7 @@
       </c>
       <c r="J47" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>1</v>
@@ -8156,14 +8269,14 @@
       </c>
       <c r="N47" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="O47" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P47" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A145',projector:'True',seats:'15')</v>
+        <v>@s1.rooms.create(description:'A145',projector:'False',seats:'18')</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -8209,14 +8322,14 @@
       </c>
       <c r="N48" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="O48" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P48" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A146',projector:'True',seats:'24')</v>
+        <v>@s1.rooms.create(description:'A146',projector:'True',seats:'28')</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -8249,7 +8362,7 @@
       </c>
       <c r="J49" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>1</v>
@@ -8262,14 +8375,14 @@
       </c>
       <c r="N49" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="O49" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P49" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>@s1.rooms.create(description:'A147',projector:'False',seats:'30')</v>
+        <v>@s1.rooms.create(description:'A147',projector:'True',seats:'15')</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -8302,7 +8415,7 @@
       </c>
       <c r="J50" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>1</v>
@@ -8315,14 +8428,14 @@
       </c>
       <c r="N50" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O50" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P50" t="str">
         <f t="shared" ref="P50" ca="1" si="3">IF(ISBLANK(F50),"",CONCATENATE(A50,B50,C50,D50,E50,F50,G50,H50,I50,J50,K50,L50,M50,N50,O50))</f>
-        <v>@s2.rooms.create(description:'A147',projector:'False',seats:'28')</v>
+        <v>@s2.rooms.create(description:'A147',projector:'True',seats:'29')</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -8355,7 +8468,7 @@
       </c>
       <c r="J51" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>1</v>
@@ -8368,14 +8481,14 @@
       </c>
       <c r="N51" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="O51" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P51" t="str">
         <f t="shared" ref="P51:P104" ca="1" si="4">IF(ISBLANK(F51),"",CONCATENATE(A51,B51,C51,D51,E51,F51,G51,H51,I51,J51,K51,L51,M51,N51,O51))</f>
-        <v>@s2.rooms.create(description:'A148',projector:'True',seats:'25')</v>
+        <v>@s2.rooms.create(description:'A148',projector:'False',seats:'15')</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -8408,7 +8521,7 @@
       </c>
       <c r="J52" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>1</v>
@@ -8421,14 +8534,14 @@
       </c>
       <c r="N52" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="O52" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P52" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A149',projector:'True',seats:'22')</v>
+        <v>@s2.rooms.create(description:'A149',projector:'False',seats:'18')</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
@@ -8474,14 +8587,14 @@
       </c>
       <c r="N53" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="O53" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P53" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A150',projector:'True',seats:'25')</v>
+        <v>@s2.rooms.create(description:'A150',projector:'True',seats:'29')</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -8514,7 +8627,7 @@
       </c>
       <c r="J54" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>1</v>
@@ -8534,7 +8647,7 @@
       </c>
       <c r="P54" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A151',projector:'False',seats:'24')</v>
+        <v>@s2.rooms.create(description:'A151',projector:'True',seats:'24')</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -8567,7 +8680,7 @@
       </c>
       <c r="J55" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>1</v>
@@ -8587,7 +8700,7 @@
       </c>
       <c r="P55" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A152',projector:'False',seats:'21')</v>
+        <v>@s2.rooms.create(description:'A152',projector:'True',seats:'21')</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -8633,14 +8746,14 @@
       </c>
       <c r="N56" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="O56" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P56" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A153',projector:'False',seats:'30')</v>
+        <v>@s2.rooms.create(description:'A153',projector:'False',seats:'26')</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -8673,7 +8786,7 @@
       </c>
       <c r="J57" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>1</v>
@@ -8693,7 +8806,7 @@
       </c>
       <c r="P57" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A154',projector:'True',seats:'24')</v>
+        <v>@s2.rooms.create(description:'A154',projector:'False',seats:'24')</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -8739,14 +8852,14 @@
       </c>
       <c r="N58" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O58" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P58" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A155',projector:'True',seats:'20')</v>
+        <v>@s2.rooms.create(description:'A155',projector:'True',seats:'21')</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -8779,7 +8892,7 @@
       </c>
       <c r="J59" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>1</v>
@@ -8792,14 +8905,14 @@
       </c>
       <c r="N59" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="O59" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P59" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A156',projector:'True',seats:'18')</v>
+        <v>@s2.rooms.create(description:'A156',projector:'False',seats:'27')</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
@@ -8832,7 +8945,7 @@
       </c>
       <c r="J60" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>1</v>
@@ -8852,7 +8965,7 @@
       </c>
       <c r="P60" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A157',projector:'False',seats:'26')</v>
+        <v>@s2.rooms.create(description:'A157',projector:'True',seats:'26')</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
@@ -8885,7 +8998,7 @@
       </c>
       <c r="J61" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>1</v>
@@ -8898,14 +9011,14 @@
       </c>
       <c r="N61" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="O61" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A158',projector:'False',seats:'24')</v>
+        <v>@s2.rooms.create(description:'A158',projector:'True',seats:'19')</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
@@ -8938,7 +9051,7 @@
       </c>
       <c r="J62" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>1</v>
@@ -8951,14 +9064,14 @@
       </c>
       <c r="N62" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="O62" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P62" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A159',projector:'False',seats:'15')</v>
+        <v>@s2.rooms.create(description:'A159',projector:'True',seats:'17')</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
@@ -8991,7 +9104,7 @@
       </c>
       <c r="J63" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>1</v>
@@ -9004,14 +9117,14 @@
       </c>
       <c r="N63" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="O63" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P63" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A160',projector:'True',seats:'20')</v>
+        <v>@s2.rooms.create(description:'A160',projector:'False',seats:'23')</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
@@ -9044,7 +9157,7 @@
       </c>
       <c r="J64" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>1</v>
@@ -9057,14 +9170,14 @@
       </c>
       <c r="N64" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="O64" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P64" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A161',projector:'False',seats:'24')</v>
+        <v>@s2.rooms.create(description:'A161',projector:'True',seats:'27')</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
@@ -9110,14 +9223,14 @@
       </c>
       <c r="N65" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="O65" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P65" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A162',projector:'True',seats:'16')</v>
+        <v>@s2.rooms.create(description:'A162',projector:'True',seats:'30')</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
@@ -9150,7 +9263,7 @@
       </c>
       <c r="J66" s="5" t="str">
         <f t="shared" ref="J66:J104" ca="1" si="5">IF(RAND()&lt;0.5,"True","False")</f>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>1</v>
@@ -9163,14 +9276,14 @@
       </c>
       <c r="N66" s="8">
         <f t="shared" ref="N66:N104" ca="1" si="6">RANDBETWEEN(15,30)</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O66" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P66" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A163',projector:'True',seats:'17')</v>
+        <v>@s2.rooms.create(description:'A163',projector:'False',seats:'16')</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
@@ -9216,14 +9329,14 @@
       </c>
       <c r="N67" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="O67" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A164',projector:'True',seats:'30')</v>
+        <v>@s2.rooms.create(description:'A164',projector:'True',seats:'23')</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
@@ -9269,14 +9382,14 @@
       </c>
       <c r="N68" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="O68" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P68" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A165',projector:'False',seats:'30')</v>
+        <v>@s2.rooms.create(description:'A165',projector:'False',seats:'25')</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
@@ -9309,7 +9422,7 @@
       </c>
       <c r="J69" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>1</v>
@@ -9322,14 +9435,14 @@
       </c>
       <c r="N69" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="O69" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P69" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A166',projector:'True',seats:'24')</v>
+        <v>@s2.rooms.create(description:'A166',projector:'False',seats:'15')</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
@@ -9362,7 +9475,7 @@
       </c>
       <c r="J70" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>1</v>
@@ -9375,14 +9488,14 @@
       </c>
       <c r="N70" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="O70" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P70" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A167',projector:'False',seats:'23')</v>
+        <v>@s2.rooms.create(description:'A167',projector:'True',seats:'29')</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
@@ -9415,7 +9528,7 @@
       </c>
       <c r="J71" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K71" s="1" t="s">
         <v>1</v>
@@ -9428,14 +9541,14 @@
       </c>
       <c r="N71" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="O71" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P71" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A168',projector:'False',seats:'16')</v>
+        <v>@s2.rooms.create(description:'A168',projector:'True',seats:'24')</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
@@ -9468,7 +9581,7 @@
       </c>
       <c r="J72" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K72" s="1" t="s">
         <v>1</v>
@@ -9488,7 +9601,7 @@
       </c>
       <c r="P72" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A169',projector:'True',seats:'22')</v>
+        <v>@s2.rooms.create(description:'A169',projector:'False',seats:'22')</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
@@ -9521,7 +9634,7 @@
       </c>
       <c r="J73" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K73" s="1" t="s">
         <v>1</v>
@@ -9534,14 +9647,14 @@
       </c>
       <c r="N73" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O73" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P73" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A170',projector:'False',seats:'18')</v>
+        <v>@s2.rooms.create(description:'A170',projector:'True',seats:'16')</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
@@ -9574,7 +9687,7 @@
       </c>
       <c r="J74" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K74" s="1" t="s">
         <v>1</v>
@@ -9587,14 +9700,14 @@
       </c>
       <c r="N74" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="O74" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P74" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A171',projector:'False',seats:'24')</v>
+        <v>@s2.rooms.create(description:'A171',projector:'True',seats:'20')</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
@@ -9627,7 +9740,7 @@
       </c>
       <c r="J75" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K75" s="1" t="s">
         <v>1</v>
@@ -9647,7 +9760,7 @@
       </c>
       <c r="P75" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A172',projector:'False',seats:'15')</v>
+        <v>@s2.rooms.create(description:'A172',projector:'True',seats:'15')</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
@@ -9693,14 +9806,14 @@
       </c>
       <c r="N76" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="O76" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P76" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A173',projector:'True',seats:'18')</v>
+        <v>@s2.rooms.create(description:'A173',projector:'True',seats:'22')</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
@@ -9746,14 +9859,14 @@
       </c>
       <c r="N77" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="O77" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P77" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A174',projector:'False',seats:'15')</v>
+        <v>@s2.rooms.create(description:'A174',projector:'False',seats:'21')</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
@@ -9799,14 +9912,14 @@
       </c>
       <c r="N78" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="O78" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P78" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A175',projector:'False',seats:'16')</v>
+        <v>@s2.rooms.create(description:'A175',projector:'False',seats:'25')</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
@@ -9852,14 +9965,14 @@
       </c>
       <c r="N79" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="O79" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P79" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A176',projector:'True',seats:'30')</v>
+        <v>@s2.rooms.create(description:'A176',projector:'True',seats:'23')</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
@@ -9892,7 +10005,7 @@
       </c>
       <c r="J80" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K80" s="1" t="s">
         <v>1</v>
@@ -9905,14 +10018,14 @@
       </c>
       <c r="N80" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="O80" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P80" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A177',projector:'False',seats:'15')</v>
+        <v>@s2.rooms.create(description:'A177',projector:'True',seats:'26')</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
@@ -9958,14 +10071,14 @@
       </c>
       <c r="N81" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="O81" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P81" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A178',projector:'False',seats:'17')</v>
+        <v>@s2.rooms.create(description:'A178',projector:'False',seats:'27')</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
@@ -9998,7 +10111,7 @@
       </c>
       <c r="J82" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K82" s="1" t="s">
         <v>1</v>
@@ -10011,14 +10124,14 @@
       </c>
       <c r="N82" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O82" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P82" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A179',projector:'True',seats:'18')</v>
+        <v>@s2.rooms.create(description:'A179',projector:'False',seats:'17')</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
@@ -10051,7 +10164,7 @@
       </c>
       <c r="J83" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K83" s="1" t="s">
         <v>1</v>
@@ -10064,14 +10177,14 @@
       </c>
       <c r="N83" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="O83" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P83" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A180',projector:'True',seats:'21')</v>
+        <v>@s2.rooms.create(description:'A180',projector:'False',seats:'26')</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
@@ -10104,7 +10217,7 @@
       </c>
       <c r="J84" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K84" s="1" t="s">
         <v>1</v>
@@ -10117,14 +10230,14 @@
       </c>
       <c r="N84" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="O84" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P84" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A181',projector:'False',seats:'17')</v>
+        <v>@s2.rooms.create(description:'A181',projector:'True',seats:'23')</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
@@ -10157,7 +10270,7 @@
       </c>
       <c r="J85" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K85" s="1" t="s">
         <v>1</v>
@@ -10177,7 +10290,7 @@
       </c>
       <c r="P85" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A182',projector:'False',seats:'18')</v>
+        <v>@s2.rooms.create(description:'A182',projector:'True',seats:'18')</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
@@ -10210,7 +10323,7 @@
       </c>
       <c r="J86" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K86" s="1" t="s">
         <v>1</v>
@@ -10223,14 +10336,14 @@
       </c>
       <c r="N86" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O86" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P86" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A183',projector:'False',seats:'27')</v>
+        <v>@s2.rooms.create(description:'A183',projector:'True',seats:'26')</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
@@ -10276,14 +10389,14 @@
       </c>
       <c r="N87" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="O87" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P87" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A184',projector:'True',seats:'22')</v>
+        <v>@s2.rooms.create(description:'A184',projector:'True',seats:'30')</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
@@ -10329,14 +10442,14 @@
       </c>
       <c r="N88" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O88" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P88" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A185',projector:'False',seats:'29')</v>
+        <v>@s2.rooms.create(description:'A185',projector:'False',seats:'30')</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
@@ -10382,14 +10495,14 @@
       </c>
       <c r="N89" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="O89" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P89" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A186',projector:'True',seats:'18')</v>
+        <v>@s2.rooms.create(description:'A186',projector:'True',seats:'21')</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
@@ -10422,7 +10535,7 @@
       </c>
       <c r="J90" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K90" s="1" t="s">
         <v>1</v>
@@ -10435,14 +10548,14 @@
       </c>
       <c r="N90" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O90" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P90" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A187',projector:'True',seats:'22')</v>
+        <v>@s2.rooms.create(description:'A187',projector:'False',seats:'24')</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
@@ -10488,14 +10601,14 @@
       </c>
       <c r="N91" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="O91" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P91" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A188',projector:'True',seats:'30')</v>
+        <v>@s2.rooms.create(description:'A188',projector:'True',seats:'23')</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
@@ -10541,14 +10654,14 @@
       </c>
       <c r="N92" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O92" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P92" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A189',projector:'True',seats:'29')</v>
+        <v>@s2.rooms.create(description:'A189',projector:'True',seats:'27')</v>
       </c>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
@@ -10594,14 +10707,14 @@
       </c>
       <c r="N93" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O93" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P93" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A190',projector:'True',seats:'25')</v>
+        <v>@s2.rooms.create(description:'A190',projector:'True',seats:'26')</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
@@ -10634,7 +10747,7 @@
       </c>
       <c r="J94" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K94" s="1" t="s">
         <v>1</v>
@@ -10647,14 +10760,14 @@
       </c>
       <c r="N94" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="O94" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P94" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A191',projector:'True',seats:'19')</v>
+        <v>@s2.rooms.create(description:'A191',projector:'False',seats:'25')</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
@@ -10700,14 +10813,14 @@
       </c>
       <c r="N95" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="O95" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P95" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A192',projector:'False',seats:'28')</v>
+        <v>@s2.rooms.create(description:'A192',projector:'False',seats:'22')</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
@@ -10753,14 +10866,14 @@
       </c>
       <c r="N96" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O96" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P96" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A193',projector:'True',seats:'28')</v>
+        <v>@s2.rooms.create(description:'A193',projector:'True',seats:'27')</v>
       </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
@@ -10793,7 +10906,7 @@
       </c>
       <c r="J97" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K97" s="1" t="s">
         <v>1</v>
@@ -10806,14 +10919,14 @@
       </c>
       <c r="N97" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="O97" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P97" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A194',projector:'False',seats:'21')</v>
+        <v>@s2.rooms.create(description:'A194',projector:'True',seats:'27')</v>
       </c>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
@@ -10846,7 +10959,7 @@
       </c>
       <c r="J98" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K98" s="1" t="s">
         <v>1</v>
@@ -10859,14 +10972,14 @@
       </c>
       <c r="N98" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="O98" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P98" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A195',projector:'False',seats:'23')</v>
+        <v>@s2.rooms.create(description:'A195',projector:'True',seats:'19')</v>
       </c>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
@@ -10912,14 +11025,14 @@
       </c>
       <c r="N99" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="O99" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P99" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A196',projector:'True',seats:'29')</v>
+        <v>@s2.rooms.create(description:'A196',projector:'True',seats:'18')</v>
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
@@ -10952,7 +11065,7 @@
       </c>
       <c r="J100" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K100" s="1" t="s">
         <v>1</v>
@@ -10965,14 +11078,14 @@
       </c>
       <c r="N100" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="O100" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P100" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A197',projector:'True',seats:'15')</v>
+        <v>@s2.rooms.create(description:'A197',projector:'False',seats:'29')</v>
       </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
@@ -11018,14 +11131,14 @@
       </c>
       <c r="N101" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O101" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P101" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A198',projector:'False',seats:'23')</v>
+        <v>@s2.rooms.create(description:'A198',projector:'False',seats:'22')</v>
       </c>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
@@ -11058,7 +11171,7 @@
       </c>
       <c r="J102" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K102" s="1" t="s">
         <v>1</v>
@@ -11071,14 +11184,14 @@
       </c>
       <c r="N102" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="O102" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P102" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A199',projector:'False',seats:'17')</v>
+        <v>@s2.rooms.create(description:'A199',projector:'True',seats:'15')</v>
       </c>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
@@ -11111,7 +11224,7 @@
       </c>
       <c r="J103" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K103" s="1" t="s">
         <v>1</v>
@@ -11124,14 +11237,14 @@
       </c>
       <c r="N103" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O103" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P103" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A200',projector:'True',seats:'29')</v>
+        <v>@s2.rooms.create(description:'A200',projector:'False',seats:'30')</v>
       </c>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
@@ -11164,7 +11277,7 @@
       </c>
       <c r="J104" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K104" s="1" t="s">
         <v>1</v>
@@ -11177,14 +11290,14 @@
       </c>
       <c r="N104" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="O104" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P104" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>@s2.rooms.create(description:'A201',projector:'True',seats:'27')</v>
+        <v>@s2.rooms.create(description:'A201',projector:'False',seats:'22')</v>
       </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
@@ -11217,7 +11330,7 @@
       </c>
       <c r="J105" s="5" t="str">
         <f t="shared" ref="J105:J159" ca="1" si="7">IF(RAND()&lt;0.5,"True","False")</f>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K105" s="1" t="s">
         <v>1</v>
@@ -11230,14 +11343,14 @@
       </c>
       <c r="N105" s="8">
         <f t="shared" ref="N105:N159" ca="1" si="8">RANDBETWEEN(15,30)</f>
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="O105" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P105" t="str">
         <f t="shared" ref="P105:P159" ca="1" si="9">IF(ISBLANK(F105),"",CONCATENATE(A105,B105,C105,D105,E105,F105,G105,H105,I105,J105,K105,L105,M105,N105,O105))</f>
-        <v>@s3.rooms.create(description:'A147',projector:'False',seats:'23')</v>
+        <v>@s3.rooms.create(description:'A147',projector:'True',seats:'30')</v>
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
@@ -11283,14 +11396,14 @@
       </c>
       <c r="N106" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="O106" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P106" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A148',projector:'True',seats:'21')</v>
+        <v>@s3.rooms.create(description:'A148',projector:'True',seats:'25')</v>
       </c>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
@@ -11323,7 +11436,7 @@
       </c>
       <c r="J107" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K107" s="1" t="s">
         <v>1</v>
@@ -11336,14 +11449,14 @@
       </c>
       <c r="N107" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O107" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P107" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A149',projector:'True',seats:'20')</v>
+        <v>@s3.rooms.create(description:'A149',projector:'False',seats:'22')</v>
       </c>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
@@ -11389,14 +11502,14 @@
       </c>
       <c r="N108" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="O108" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P108" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A150',projector:'True',seats:'26')</v>
+        <v>@s3.rooms.create(description:'A150',projector:'True',seats:'17')</v>
       </c>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
@@ -11442,14 +11555,14 @@
       </c>
       <c r="N109" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="O109" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P109" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A151',projector:'False',seats:'28')</v>
+        <v>@s3.rooms.create(description:'A151',projector:'False',seats:'24')</v>
       </c>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
@@ -11482,7 +11595,7 @@
       </c>
       <c r="J110" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K110" s="1" t="s">
         <v>1</v>
@@ -11495,14 +11608,14 @@
       </c>
       <c r="N110" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O110" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P110" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A152',projector:'True',seats:'22')</v>
+        <v>@s3.rooms.create(description:'A152',projector:'False',seats:'23')</v>
       </c>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
@@ -11548,14 +11661,14 @@
       </c>
       <c r="N111" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="O111" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P111" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A153',projector:'True',seats:'20')</v>
+        <v>@s3.rooms.create(description:'A153',projector:'True',seats:'25')</v>
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
@@ -11641,7 +11754,7 @@
       </c>
       <c r="J113" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K113" s="1" t="s">
         <v>1</v>
@@ -11654,14 +11767,14 @@
       </c>
       <c r="N113" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="O113" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P113" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A155',projector:'True',seats:'18')</v>
+        <v>@s3.rooms.create(description:'A155',projector:'False',seats:'21')</v>
       </c>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.25">
@@ -11707,14 +11820,14 @@
       </c>
       <c r="N114" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="O114" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P114" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A156',projector:'True',seats:'28')</v>
+        <v>@s3.rooms.create(description:'A156',projector:'True',seats:'30')</v>
       </c>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.25">
@@ -11747,7 +11860,7 @@
       </c>
       <c r="J115" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K115" s="1" t="s">
         <v>1</v>
@@ -11760,14 +11873,14 @@
       </c>
       <c r="N115" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="O115" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P115" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A157',projector:'False',seats:'21')</v>
+        <v>@s3.rooms.create(description:'A157',projector:'True',seats:'16')</v>
       </c>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.25">
@@ -11800,7 +11913,7 @@
       </c>
       <c r="J116" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K116" s="1" t="s">
         <v>1</v>
@@ -11813,14 +11926,14 @@
       </c>
       <c r="N116" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="O116" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P116" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A158',projector:'False',seats:'17')</v>
+        <v>@s3.rooms.create(description:'A158',projector:'True',seats:'23')</v>
       </c>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
@@ -11853,7 +11966,7 @@
       </c>
       <c r="J117" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K117" s="1" t="s">
         <v>1</v>
@@ -11866,14 +11979,14 @@
       </c>
       <c r="N117" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="O117" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P117" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A159',projector:'False',seats:'17')</v>
+        <v>@s3.rooms.create(description:'A159',projector:'True',seats:'26')</v>
       </c>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.25">
@@ -11919,14 +12032,14 @@
       </c>
       <c r="N118" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="O118" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P118" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A160',projector:'False',seats:'15')</v>
+        <v>@s3.rooms.create(description:'A160',projector:'False',seats:'30')</v>
       </c>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.25">
@@ -11972,14 +12085,14 @@
       </c>
       <c r="N119" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="O119" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P119" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A161',projector:'False',seats:'16')</v>
+        <v>@s3.rooms.create(description:'A161',projector:'False',seats:'27')</v>
       </c>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.25">
@@ -12065,7 +12178,7 @@
       </c>
       <c r="J121" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K121" s="1" t="s">
         <v>1</v>
@@ -12078,14 +12191,14 @@
       </c>
       <c r="N121" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="O121" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P121" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A163',projector:'True',seats:'28')</v>
+        <v>@s3.rooms.create(description:'A163',projector:'False',seats:'16')</v>
       </c>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.25">
@@ -12118,7 +12231,7 @@
       </c>
       <c r="J122" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K122" s="1" t="s">
         <v>1</v>
@@ -12131,14 +12244,14 @@
       </c>
       <c r="N122" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="O122" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P122" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A164',projector:'False',seats:'22')</v>
+        <v>@s3.rooms.create(description:'A164',projector:'True',seats:'16')</v>
       </c>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.25">
@@ -12171,7 +12284,7 @@
       </c>
       <c r="J123" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K123" s="1" t="s">
         <v>1</v>
@@ -12184,14 +12297,14 @@
       </c>
       <c r="N123" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="O123" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P123" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A165',projector:'True',seats:'15')</v>
+        <v>@s3.rooms.create(description:'A165',projector:'False',seats:'29')</v>
       </c>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.25">
@@ -12224,7 +12337,7 @@
       </c>
       <c r="J124" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K124" s="1" t="s">
         <v>1</v>
@@ -12237,14 +12350,14 @@
       </c>
       <c r="N124" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="O124" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P124" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A166',projector:'True',seats:'17')</v>
+        <v>@s3.rooms.create(description:'A166',projector:'False',seats:'30')</v>
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
@@ -12277,7 +12390,7 @@
       </c>
       <c r="J125" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K125" s="1" t="s">
         <v>1</v>
@@ -12290,14 +12403,14 @@
       </c>
       <c r="N125" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="O125" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P125" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A167',projector:'True',seats:'26')</v>
+        <v>@s3.rooms.create(description:'A167',projector:'False',seats:'21')</v>
       </c>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.25">
@@ -12330,7 +12443,7 @@
       </c>
       <c r="J126" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K126" s="1" t="s">
         <v>1</v>
@@ -12343,14 +12456,14 @@
       </c>
       <c r="N126" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="O126" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P126" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A168',projector:'False',seats:'15')</v>
+        <v>@s3.rooms.create(description:'A168',projector:'True',seats:'20')</v>
       </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.25">
@@ -12383,7 +12496,7 @@
       </c>
       <c r="J127" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K127" s="1" t="s">
         <v>1</v>
@@ -12396,14 +12509,14 @@
       </c>
       <c r="N127" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="O127" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P127" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A169',projector:'True',seats:'30')</v>
+        <v>@s3.rooms.create(description:'A169',projector:'False',seats:'27')</v>
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.25">
@@ -12436,7 +12549,7 @@
       </c>
       <c r="J128" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K128" s="1" t="s">
         <v>1</v>
@@ -12449,14 +12562,14 @@
       </c>
       <c r="N128" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O128" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P128" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A170',projector:'True',seats:'22')</v>
+        <v>@s3.rooms.create(description:'A170',projector:'False',seats:'15')</v>
       </c>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.25">
@@ -12502,14 +12615,14 @@
       </c>
       <c r="N129" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="O129" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P129" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A171',projector:'False',seats:'18')</v>
+        <v>@s3.rooms.create(description:'A171',projector:'False',seats:'21')</v>
       </c>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.25">
@@ -12542,7 +12655,7 @@
       </c>
       <c r="J130" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K130" s="1" t="s">
         <v>1</v>
@@ -12555,14 +12668,14 @@
       </c>
       <c r="N130" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="O130" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P130" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A172',projector:'False',seats:'19')</v>
+        <v>@s3.rooms.create(description:'A172',projector:'True',seats:'26')</v>
       </c>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.25">
@@ -12595,7 +12708,7 @@
       </c>
       <c r="J131" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K131" s="1" t="s">
         <v>1</v>
@@ -12608,14 +12721,14 @@
       </c>
       <c r="N131" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="O131" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P131" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A173',projector:'False',seats:'22')</v>
+        <v>@s3.rooms.create(description:'A173',projector:'True',seats:'28')</v>
       </c>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.25">
@@ -12714,14 +12827,14 @@
       </c>
       <c r="N133" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="O133" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P133" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A175',projector:'False',seats:'18')</v>
+        <v>@s3.rooms.create(description:'A175',projector:'False',seats:'24')</v>
       </c>
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.25">
@@ -12754,7 +12867,7 @@
       </c>
       <c r="J134" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K134" s="1" t="s">
         <v>1</v>
@@ -12767,14 +12880,14 @@
       </c>
       <c r="N134" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O134" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P134" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A176',projector:'False',seats:'29')</v>
+        <v>@s3.rooms.create(description:'A176',projector:'True',seats:'30')</v>
       </c>
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.25">
@@ -12807,7 +12920,7 @@
       </c>
       <c r="J135" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K135" s="1" t="s">
         <v>1</v>
@@ -12820,14 +12933,14 @@
       </c>
       <c r="N135" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="O135" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P135" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A177',projector:'True',seats:'16')</v>
+        <v>@s3.rooms.create(description:'A177',projector:'False',seats:'28')</v>
       </c>
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.25">
@@ -12873,14 +12986,14 @@
       </c>
       <c r="N136" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="O136" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P136" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A178',projector:'False',seats:'23')</v>
+        <v>@s3.rooms.create(description:'A178',projector:'False',seats:'19')</v>
       </c>
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.25">
@@ -12913,7 +13026,7 @@
       </c>
       <c r="J137" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K137" s="1" t="s">
         <v>1</v>
@@ -12926,14 +13039,14 @@
       </c>
       <c r="N137" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="O137" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P137" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A179',projector:'False',seats:'17')</v>
+        <v>@s3.rooms.create(description:'A179',projector:'True',seats:'29')</v>
       </c>
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.25">
@@ -12966,7 +13079,7 @@
       </c>
       <c r="J138" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K138" s="1" t="s">
         <v>1</v>
@@ -12979,14 +13092,14 @@
       </c>
       <c r="N138" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="O138" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P138" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A180',projector:'True',seats:'17')</v>
+        <v>@s3.rooms.create(description:'A180',projector:'False',seats:'28')</v>
       </c>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.25">
@@ -13032,14 +13145,14 @@
       </c>
       <c r="N139" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="O139" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P139" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A181',projector:'False',seats:'27')</v>
+        <v>@s3.rooms.create(description:'A181',projector:'False',seats:'20')</v>
       </c>
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.25">
@@ -13072,7 +13185,7 @@
       </c>
       <c r="J140" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K140" s="1" t="s">
         <v>1</v>
@@ -13085,14 +13198,14 @@
       </c>
       <c r="N140" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="O140" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P140" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A182',projector:'True',seats:'20')</v>
+        <v>@s3.rooms.create(description:'A182',projector:'False',seats:'15')</v>
       </c>
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.25">
@@ -13138,14 +13251,14 @@
       </c>
       <c r="N141" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="O141" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P141" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A183',projector:'False',seats:'16')</v>
+        <v>@s3.rooms.create(description:'A183',projector:'False',seats:'24')</v>
       </c>
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.25">
@@ -13178,7 +13291,7 @@
       </c>
       <c r="J142" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K142" s="1" t="s">
         <v>1</v>
@@ -13198,7 +13311,7 @@
       </c>
       <c r="P142" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A184',projector:'True',seats:'28')</v>
+        <v>@s3.rooms.create(description:'A184',projector:'False',seats:'28')</v>
       </c>
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.25">
@@ -13284,7 +13397,7 @@
       </c>
       <c r="J144" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K144" s="1" t="s">
         <v>1</v>
@@ -13297,14 +13410,14 @@
       </c>
       <c r="N144" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="O144" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P144" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A186',projector:'True',seats:'30')</v>
+        <v>@s3.rooms.create(description:'A186',projector:'False',seats:'20')</v>
       </c>
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.25">
@@ -13350,14 +13463,14 @@
       </c>
       <c r="N145" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="O145" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P145" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A187',projector:'False',seats:'24')</v>
+        <v>@s3.rooms.create(description:'A187',projector:'False',seats:'27')</v>
       </c>
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.25">
@@ -13390,7 +13503,7 @@
       </c>
       <c r="J146" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K146" s="1" t="s">
         <v>1</v>
@@ -13403,14 +13516,14 @@
       </c>
       <c r="N146" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="O146" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P146" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A188',projector:'False',seats:'19')</v>
+        <v>@s3.rooms.create(description:'A188',projector:'True',seats:'28')</v>
       </c>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.25">
@@ -13443,7 +13556,7 @@
       </c>
       <c r="J147" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K147" s="1" t="s">
         <v>1</v>
@@ -13456,14 +13569,14 @@
       </c>
       <c r="N147" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O147" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P147" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A189',projector:'True',seats:'26')</v>
+        <v>@s3.rooms.create(description:'A189',projector:'False',seats:'24')</v>
       </c>
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.25">
@@ -13509,14 +13622,14 @@
       </c>
       <c r="N148" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="O148" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P148" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A190',projector:'False',seats:'26')</v>
+        <v>@s3.rooms.create(description:'A190',projector:'False',seats:'28')</v>
       </c>
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.25">
@@ -13549,7 +13662,7 @@
       </c>
       <c r="J149" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K149" s="1" t="s">
         <v>1</v>
@@ -13562,14 +13675,14 @@
       </c>
       <c r="N149" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="O149" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P149" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A191',projector:'False',seats:'30')</v>
+        <v>@s3.rooms.create(description:'A191',projector:'True',seats:'18')</v>
       </c>
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.25">
@@ -13615,14 +13728,14 @@
       </c>
       <c r="N150" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="O150" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P150" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A192',projector:'True',seats:'29')</v>
+        <v>@s3.rooms.create(description:'A192',projector:'True',seats:'16')</v>
       </c>
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.25">
@@ -13668,14 +13781,14 @@
       </c>
       <c r="N151" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="O151" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P151" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A193',projector:'True',seats:'15')</v>
+        <v>@s3.rooms.create(description:'A193',projector:'True',seats:'22')</v>
       </c>
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.25">
@@ -13721,14 +13834,14 @@
       </c>
       <c r="N152" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="O152" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P152" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A194',projector:'True',seats:'17')</v>
+        <v>@s3.rooms.create(description:'A194',projector:'True',seats:'24')</v>
       </c>
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.25">
@@ -13774,14 +13887,14 @@
       </c>
       <c r="N153" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="O153" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P153" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A195',projector:'True',seats:'17')</v>
+        <v>@s3.rooms.create(description:'A195',projector:'True',seats:'22')</v>
       </c>
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.25">
@@ -13827,14 +13940,14 @@
       </c>
       <c r="N154" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="O154" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P154" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A196',projector:'False',seats:'15')</v>
+        <v>@s3.rooms.create(description:'A196',projector:'False',seats:'23')</v>
       </c>
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.25">
@@ -13880,14 +13993,14 @@
       </c>
       <c r="N155" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="O155" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P155" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A197',projector:'True',seats:'19')</v>
+        <v>@s3.rooms.create(description:'A197',projector:'True',seats:'15')</v>
       </c>
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.25">
@@ -13920,7 +14033,7 @@
       </c>
       <c r="J156" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>False</v>
+        <v>True</v>
       </c>
       <c r="K156" s="1" t="s">
         <v>1</v>
@@ -13940,7 +14053,7 @@
       </c>
       <c r="P156" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A198',projector:'False',seats:'24')</v>
+        <v>@s3.rooms.create(description:'A198',projector:'True',seats:'24')</v>
       </c>
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.25">
@@ -13986,14 +14099,14 @@
       </c>
       <c r="N157" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="O157" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P157" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A199',projector:'False',seats:'26')</v>
+        <v>@s3.rooms.create(description:'A199',projector:'False',seats:'18')</v>
       </c>
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.25">
@@ -14026,7 +14139,7 @@
       </c>
       <c r="J158" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>True</v>
+        <v>False</v>
       </c>
       <c r="K158" s="1" t="s">
         <v>1</v>
@@ -14039,14 +14152,14 @@
       </c>
       <c r="N158" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="O158" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P158" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A200',projector:'True',seats:'29')</v>
+        <v>@s3.rooms.create(description:'A200',projector:'False',seats:'21')</v>
       </c>
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.25">
@@ -14092,14 +14205,14 @@
       </c>
       <c r="N159" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="O159" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P159" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>@s3.rooms.create(description:'A201',projector:'True',seats:'15')</v>
+        <v>@s3.rooms.create(description:'A201',projector:'True',seats:'27')</v>
       </c>
     </row>
   </sheetData>
@@ -14320,8 +14433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q87"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O87"/>
+    <sheetView topLeftCell="J2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18579,7 +18692,7 @@
   <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J31"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21282,8 +21395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21933,10 +22046,777 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:V12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2:V12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="1.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="1.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3" customWidth="1"/>
+    <col min="21" max="21" width="1.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="94.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>478</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>480</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>236</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>477</v>
+      </c>
+      <c r="O2" t="s">
+        <v>239</v>
+      </c>
+      <c r="P2">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="R2" t="s">
+        <v>512</v>
+      </c>
+      <c r="S2" t="s">
+        <v>239</v>
+      </c>
+      <c r="T2" s="6"/>
+      <c r="U2" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="V2" s="13" t="str">
+        <f>IF(ISBLANK(G2),"",CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2,R2,S2,T2,Discipline!A2&amp;Discipline!B2,U2))</f>
+        <v>@project1 = Project.create(name:'Prj1',description:'Descr Proj 1',grade:10,discipline:@discipline1)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>481</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>482</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>236</v>
+      </c>
+      <c r="K3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>477</v>
+      </c>
+      <c r="O3" t="s">
+        <v>239</v>
+      </c>
+      <c r="P3">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="R3" t="s">
+        <v>512</v>
+      </c>
+      <c r="S3" t="s">
+        <v>239</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="V3" s="13" t="str">
+        <f>IF(ISBLANK(G3),"",CONCATENATE(A3,B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3,M3,N3,O3,P3,Q3,R3,S3,T3,Discipline!A3&amp;Discipline!B3,U3))</f>
+        <v>@project2 = Project.create(name:'Prj2',description:'Descr Proj 2',grade:10,discipline:@discipline2)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>484</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>485</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>236</v>
+      </c>
+      <c r="K4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>477</v>
+      </c>
+      <c r="O4" t="s">
+        <v>239</v>
+      </c>
+      <c r="P4">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="R4" t="s">
+        <v>512</v>
+      </c>
+      <c r="S4" t="s">
+        <v>239</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="V4" s="13" t="str">
+        <f>IF(ISBLANK(G4),"",CONCATENATE(A4,B4,C4,D4,E4,F4,G4,H4,I4,J4,K4,L4,M4,N4,O4,P4,Q4,R4,S4,T4,Discipline!A4&amp;Discipline!B4,U4))</f>
+        <v>@project3 = Project.create(name:'Prj3',description:'Descr Proj 3',grade:10,discipline:@discipline3)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>488</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>236</v>
+      </c>
+      <c r="K5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" t="s">
+        <v>477</v>
+      </c>
+      <c r="O5" t="s">
+        <v>239</v>
+      </c>
+      <c r="P5">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="R5" t="s">
+        <v>512</v>
+      </c>
+      <c r="S5" t="s">
+        <v>239</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="V5" s="13" t="str">
+        <f>IF(ISBLANK(G5),"",CONCATENATE(A5,B5,C5,D5,E5,F5,G5,H5,I5,J5,K5,L5,M5,N5,O5,P5,Q5,R5,S5,T5,Discipline!A5&amp;Discipline!B5,U5))</f>
+        <v>@project4 = Project.create(name:'Prj4',description:'Descr Proj 4',grade:10,discipline:@discipline4)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>490</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>491</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>236</v>
+      </c>
+      <c r="K6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
+        <v>477</v>
+      </c>
+      <c r="O6" t="s">
+        <v>239</v>
+      </c>
+      <c r="P6">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="R6" t="s">
+        <v>512</v>
+      </c>
+      <c r="S6" t="s">
+        <v>239</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="V6" s="13" t="str">
+        <f>IF(ISBLANK(G6),"",CONCATENATE(A6,B6,C6,D6,E6,F6,G6,H6,I6,J6,K6,L6,M6,N6,O6,P6,Q6,R6,S6,T6,Discipline!A6&amp;Discipline!B6,U6))</f>
+        <v>@project5 = Project.create(name:'Prj5',description:'Descr Proj 5',grade:10,discipline:@discipline5)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>493</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>494</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>236</v>
+      </c>
+      <c r="K7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" t="s">
+        <v>477</v>
+      </c>
+      <c r="O7" t="s">
+        <v>239</v>
+      </c>
+      <c r="P7">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="R7" t="s">
+        <v>512</v>
+      </c>
+      <c r="S7" t="s">
+        <v>239</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="V7" s="13" t="str">
+        <f>IF(ISBLANK(G7),"",CONCATENATE(A7,B7,C7,D7,E7,F7,G7,H7,I7,J7,K7,L7,M7,N7,O7,P7,Q7,R7,S7,T7,Discipline!A7&amp;Discipline!B7,U7))</f>
+        <v>@project6 = Project.create(name:'Prj6',description:'Descr Proj 6',grade:10,discipline:@discipline6)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>496</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>497</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>236</v>
+      </c>
+      <c r="K8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" t="s">
+        <v>477</v>
+      </c>
+      <c r="O8" t="s">
+        <v>239</v>
+      </c>
+      <c r="P8">
+        <v>10</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="R8" t="s">
+        <v>512</v>
+      </c>
+      <c r="S8" t="s">
+        <v>239</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="V8" s="13" t="str">
+        <f>IF(ISBLANK(G8),"",CONCATENATE(A8,B8,C8,D8,E8,F8,G8,H8,I8,J8,K8,L8,M8,N8,O8,P8,Q8,R8,S8,T8,Discipline!A8&amp;Discipline!B8,U8))</f>
+        <v>@project7 = Project.create(name:'Prj7',description:'Descr Proj 7',grade:10,discipline:@discipline7)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>499</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>500</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>236</v>
+      </c>
+      <c r="K9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" t="s">
+        <v>477</v>
+      </c>
+      <c r="O9" t="s">
+        <v>239</v>
+      </c>
+      <c r="P9">
+        <v>10</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="R9" t="s">
+        <v>512</v>
+      </c>
+      <c r="S9" t="s">
+        <v>239</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="V9" s="13" t="str">
+        <f>IF(ISBLANK(G9),"",CONCATENATE(A9,B9,C9,D9,E9,F9,G9,H9,I9,J9,K9,L9,M9,N9,O9,P9,Q9,R9,S9,T9,Discipline!A9&amp;Discipline!B9,U9))</f>
+        <v>@project8 = Project.create(name:'Prj8',description:'Descr Proj 8',grade:10,discipline:@discipline8)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>503</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>236</v>
+      </c>
+      <c r="K10" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" t="s">
+        <v>477</v>
+      </c>
+      <c r="O10" t="s">
+        <v>239</v>
+      </c>
+      <c r="P10">
+        <v>10</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="R10" t="s">
+        <v>512</v>
+      </c>
+      <c r="S10" t="s">
+        <v>239</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="V10" s="13" t="str">
+        <f>IF(ISBLANK(G10),"",CONCATENATE(A10,B10,C10,D10,E10,F10,G10,H10,I10,J10,K10,L10,M10,N10,O10,P10,Q10,R10,S10,T10,Discipline!A10&amp;Discipline!B10,U10))</f>
+        <v>@project9 = Project.create(name:'Prj9',description:'Descr Proj 9',grade:10,discipline:@discipline9)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>505</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>506</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>236</v>
+      </c>
+      <c r="K11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
+        <v>477</v>
+      </c>
+      <c r="O11" t="s">
+        <v>239</v>
+      </c>
+      <c r="P11">
+        <v>10</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="R11" t="s">
+        <v>512</v>
+      </c>
+      <c r="S11" t="s">
+        <v>239</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="V11" s="13" t="str">
+        <f>IF(ISBLANK(G11),"",CONCATENATE(A11,B11,C11,D11,E11,F11,G11,H11,I11,J11,K11,L11,M11,N11,O11,P11,Q11,R11,S11,T11,Discipline!A11&amp;Discipline!B11,U11))</f>
+        <v>@project10 = Project.create(name:'Prj10',description:'Descr Proj 10',grade:10,discipline:@discipline10)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>508</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>509</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>236</v>
+      </c>
+      <c r="K12" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N12" t="s">
+        <v>477</v>
+      </c>
+      <c r="O12" t="s">
+        <v>239</v>
+      </c>
+      <c r="P12">
+        <v>10</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="R12" t="s">
+        <v>512</v>
+      </c>
+      <c r="S12" t="s">
+        <v>239</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="V12" s="13" t="str">
+        <f>IF(ISBLANK(G12),"",CONCATENATE(A12,B12,C12,D12,E12,F12,G12,H12,I12,J12,K12,L12,M12,N12,O12,P12,Q12,R12,S12,T12,Discipline!A12&amp;Discipline!B12,U12))</f>
+        <v>@project11 = Project.create(name:'Prj11',description:'Descr Proj 11',grade:10,discipline:@discipline11)</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH38"/>
   <sheetViews>
     <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="W31" sqref="W31"/>
+      <selection activeCell="AH3" sqref="AH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>